<commit_message>
selesai preprocessing data utama (data satudata & bmkg)
</commit_message>
<xml_diff>
--- a/Meteorological Kemayoran/kemayoran 2021 - 2024.xlsx
+++ b/Meteorological Kemayoran/kemayoran 2021 - 2024.xlsx
@@ -1,26 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kuliah\Skripsi\Meteorological Kemayoran\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD124FE-8976-4022-97D7-337ADA5F0E95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC964C1D-79EB-4D06-8F86-0DA99441E5C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2021" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2021'!$A$1:$J$1462</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5769" uniqueCount="1463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5861" uniqueCount="1527">
   <si>
     <t>Tanggal</t>
   </si>
@@ -4409,6 +4412,198 @@
   </si>
   <si>
     <t>DDD_CAR</t>
+  </si>
+  <si>
+    <t>11-12-2024</t>
+  </si>
+  <si>
+    <t>12-12-2024</t>
+  </si>
+  <si>
+    <t>13-12-2024</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>14-12-2024</t>
+  </si>
+  <si>
+    <t>15-12-2024</t>
+  </si>
+  <si>
+    <t>16-12-2024</t>
+  </si>
+  <si>
+    <t>17-12-2024</t>
+  </si>
+  <si>
+    <t>18-12-2024</t>
+  </si>
+  <si>
+    <t>19-12-2024</t>
+  </si>
+  <si>
+    <t>20-12-2024</t>
+  </si>
+  <si>
+    <t>21-12-2024</t>
+  </si>
+  <si>
+    <t>22-12-2024</t>
+  </si>
+  <si>
+    <t>23-12-2024</t>
+  </si>
+  <si>
+    <t>24-12-2024</t>
+  </si>
+  <si>
+    <t>25-12-2024</t>
+  </si>
+  <si>
+    <t>26-12-2024</t>
+  </si>
+  <si>
+    <t>27-12-2024</t>
+  </si>
+  <si>
+    <t>28-12-2024</t>
+  </si>
+  <si>
+    <t>29-12-2024</t>
+  </si>
+  <si>
+    <t>30-12-2024</t>
+  </si>
+  <si>
+    <t>31-12-2024</t>
+  </si>
+  <si>
+    <t>-6.155560</t>
+  </si>
+  <si>
+    <t>106.85</t>
+  </si>
+  <si>
+    <t>-6.155561</t>
+  </si>
+  <si>
+    <t>106.86</t>
+  </si>
+  <si>
+    <t>-6.155562</t>
+  </si>
+  <si>
+    <t>106.87</t>
+  </si>
+  <si>
+    <t>-6.155563</t>
+  </si>
+  <si>
+    <t>106.88</t>
+  </si>
+  <si>
+    <t>-6.155564</t>
+  </si>
+  <si>
+    <t>106.89</t>
+  </si>
+  <si>
+    <t>-6.155565</t>
+  </si>
+  <si>
+    <t>106.90</t>
+  </si>
+  <si>
+    <t>-6.155566</t>
+  </si>
+  <si>
+    <t>106.91</t>
+  </si>
+  <si>
+    <t>-6.155567</t>
+  </si>
+  <si>
+    <t>106.92</t>
+  </si>
+  <si>
+    <t>-6.155568</t>
+  </si>
+  <si>
+    <t>106.93</t>
+  </si>
+  <si>
+    <t>-6.155569</t>
+  </si>
+  <si>
+    <t>106.94</t>
+  </si>
+  <si>
+    <t>-6.155570</t>
+  </si>
+  <si>
+    <t>106.95</t>
+  </si>
+  <si>
+    <t>-6.155571</t>
+  </si>
+  <si>
+    <t>106.96</t>
+  </si>
+  <si>
+    <t>-6.155572</t>
+  </si>
+  <si>
+    <t>106.97</t>
+  </si>
+  <si>
+    <t>-6.155573</t>
+  </si>
+  <si>
+    <t>106.98</t>
+  </si>
+  <si>
+    <t>-6.155574</t>
+  </si>
+  <si>
+    <t>106.99</t>
+  </si>
+  <si>
+    <t>-6.155575</t>
+  </si>
+  <si>
+    <t>106.100</t>
+  </si>
+  <si>
+    <t>-6.155576</t>
+  </si>
+  <si>
+    <t>106.101</t>
+  </si>
+  <si>
+    <t>-6.155577</t>
+  </si>
+  <si>
+    <t>106.102</t>
+  </si>
+  <si>
+    <t>-6.155578</t>
+  </si>
+  <si>
+    <t>106.103</t>
+  </si>
+  <si>
+    <t>-6.155579</t>
+  </si>
+  <si>
+    <t>106.104</t>
+  </si>
+  <si>
+    <t>-6.155580</t>
+  </si>
+  <si>
+    <t>106.105</t>
   </si>
 </sst>
 </file>
@@ -4489,7 +4684,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4508,9 +4703,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4817,10 +5009,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1442"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:J1462"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4896,7 +5089,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -4928,7 +5121,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -4958,7 +5151,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -5084,7 +5277,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -5180,7 +5373,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
@@ -5210,7 +5403,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
@@ -5240,7 +5433,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -5272,7 +5465,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
@@ -5304,7 +5497,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
@@ -5336,7 +5529,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
@@ -5366,7 +5559,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
@@ -5398,7 +5591,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>23</v>
       </c>
@@ -5430,7 +5623,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>24</v>
       </c>
@@ -5462,7 +5655,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>25</v>
       </c>
@@ -5558,7 +5751,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>28</v>
       </c>
@@ -5654,7 +5847,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>31</v>
       </c>
@@ -5686,7 +5879,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>32</v>
       </c>
@@ -5718,7 +5911,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>33</v>
       </c>
@@ -5782,7 +5975,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>35</v>
       </c>
@@ -5846,7 +6039,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>37</v>
       </c>
@@ -5878,7 +6071,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>1341</v>
       </c>
@@ -5942,7 +6135,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>1343</v>
       </c>
@@ -5974,7 +6167,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>1344</v>
       </c>
@@ -6006,7 +6199,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>1345</v>
       </c>
@@ -6038,7 +6231,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>1346</v>
       </c>
@@ -6070,7 +6263,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>1347</v>
       </c>
@@ -6134,7 +6327,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>1349</v>
       </c>
@@ -6166,7 +6359,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>1350</v>
       </c>
@@ -6198,7 +6391,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>1351</v>
       </c>
@@ -6230,7 +6423,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>1352</v>
       </c>
@@ -6294,7 +6487,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>1354</v>
       </c>
@@ -6390,7 +6583,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>1357</v>
       </c>
@@ -6422,7 +6615,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>1358</v>
       </c>
@@ -6454,7 +6647,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>1359</v>
       </c>
@@ -6486,7 +6679,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>1360</v>
       </c>
@@ -6518,7 +6711,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>1361</v>
       </c>
@@ -6550,7 +6743,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>1362</v>
       </c>
@@ -6582,7 +6775,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>1363</v>
       </c>
@@ -6614,7 +6807,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>1364</v>
       </c>
@@ -6710,7 +6903,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>1367</v>
       </c>
@@ -6740,7 +6933,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>1368</v>
       </c>
@@ -6868,7 +7061,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>39</v>
       </c>
@@ -6932,7 +7125,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>41</v>
       </c>
@@ -6964,7 +7157,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>42</v>
       </c>
@@ -7028,7 +7221,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>44</v>
       </c>
@@ -7092,7 +7285,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>46</v>
       </c>
@@ -7124,7 +7317,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>47</v>
       </c>
@@ -7250,7 +7443,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>51</v>
       </c>
@@ -7314,7 +7507,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>53</v>
       </c>
@@ -7346,7 +7539,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>54</v>
       </c>
@@ -7376,7 +7569,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>55</v>
       </c>
@@ -7408,7 +7601,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>56</v>
       </c>
@@ -7438,7 +7631,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>57</v>
       </c>
@@ -7470,7 +7663,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>58</v>
       </c>
@@ -7530,7 +7723,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>60</v>
       </c>
@@ -7562,7 +7755,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>61</v>
       </c>
@@ -7626,7 +7819,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>63</v>
       </c>
@@ -7688,7 +7881,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>65</v>
       </c>
@@ -7752,7 +7945,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>67</v>
       </c>
@@ -7846,7 +8039,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>70</v>
       </c>
@@ -7876,7 +8069,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>71</v>
       </c>
@@ -7906,7 +8099,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>72</v>
       </c>
@@ -7970,7 +8163,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>74</v>
       </c>
@@ -8064,7 +8257,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>77</v>
       </c>
@@ -8380,7 +8573,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>87</v>
       </c>
@@ -8442,7 +8635,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>89</v>
       </c>
@@ -8504,7 +8697,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>91</v>
       </c>
@@ -8724,7 +8917,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>98</v>
       </c>
@@ -8816,7 +9009,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>101</v>
       </c>
@@ -8880,7 +9073,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>103</v>
       </c>
@@ -8976,7 +9169,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>106</v>
       </c>
@@ -9036,7 +9229,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>108</v>
       </c>
@@ -9068,7 +9261,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>109</v>
       </c>
@@ -9160,7 +9353,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>112</v>
       </c>
@@ -9254,7 +9447,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>115</v>
       </c>
@@ -9440,7 +9633,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>121</v>
       </c>
@@ -9504,7 +9697,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>123</v>
       </c>
@@ -9848,7 +10041,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
         <v>134</v>
       </c>
@@ -9910,7 +10103,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
         <v>136</v>
       </c>
@@ -10006,7 +10199,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
         <v>139</v>
       </c>
@@ -10070,7 +10263,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>141</v>
       </c>
@@ -10260,7 +10453,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
         <v>147</v>
       </c>
@@ -10514,7 +10707,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
         <v>155</v>
       </c>
@@ -10858,7 +11051,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
         <v>166</v>
       </c>
@@ -10888,7 +11081,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
         <v>167</v>
       </c>
@@ -10950,7 +11143,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
         <v>169</v>
       </c>
@@ -11200,7 +11393,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
         <v>177</v>
       </c>
@@ -11264,7 +11457,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
         <v>179</v>
       </c>
@@ -11452,7 +11645,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
         <v>185</v>
       </c>
@@ -11514,7 +11707,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
         <v>187</v>
       </c>
@@ -11544,7 +11737,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
         <v>188</v>
       </c>
@@ -11576,7 +11769,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
         <v>189</v>
       </c>
@@ -11608,7 +11801,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
         <v>190</v>
       </c>
@@ -11638,7 +11831,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
         <v>191</v>
       </c>
@@ -11700,7 +11893,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
         <v>193</v>
       </c>
@@ -11732,7 +11925,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
         <v>194</v>
       </c>
@@ -11762,7 +11955,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
         <v>195</v>
       </c>
@@ -11792,7 +11985,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
         <v>196</v>
       </c>
@@ -11856,7 +12049,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
         <v>198</v>
       </c>
@@ -11888,7 +12081,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
         <v>199</v>
       </c>
@@ -11950,7 +12143,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
         <v>201</v>
       </c>
@@ -11982,7 +12175,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
         <v>202</v>
       </c>
@@ -12012,7 +12205,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
         <v>203</v>
       </c>
@@ -12074,7 +12267,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
         <v>205</v>
       </c>
@@ -12106,7 +12299,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" s="2" t="s">
         <v>206</v>
       </c>
@@ -12136,7 +12329,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
         <v>207</v>
       </c>
@@ -12166,7 +12359,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
         <v>208</v>
       </c>
@@ -12258,7 +12451,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" s="2" t="s">
         <v>211</v>
       </c>
@@ -12320,7 +12513,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" s="2" t="s">
         <v>213</v>
       </c>
@@ -12444,7 +12637,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" s="2" t="s">
         <v>217</v>
       </c>
@@ -12628,7 +12821,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" s="2" t="s">
         <v>223</v>
       </c>
@@ -12658,7 +12851,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" s="2" t="s">
         <v>224</v>
       </c>
@@ -12722,7 +12915,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" s="2" t="s">
         <v>226</v>
       </c>
@@ -12882,7 +13075,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257" s="2" t="s">
         <v>231</v>
       </c>
@@ -12944,7 +13137,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
         <v>233</v>
       </c>
@@ -12976,7 +13169,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
         <v>234</v>
       </c>
@@ -13006,7 +13199,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261" s="2" t="s">
         <v>235</v>
       </c>
@@ -13190,7 +13383,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267" s="2" t="s">
         <v>241</v>
       </c>
@@ -13222,7 +13415,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268" s="2" t="s">
         <v>242</v>
       </c>
@@ -13252,7 +13445,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269" s="2" t="s">
         <v>243</v>
       </c>
@@ -13282,7 +13475,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270" s="2" t="s">
         <v>244</v>
       </c>
@@ -13346,7 +13539,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272" s="2" t="s">
         <v>246</v>
       </c>
@@ -13378,7 +13571,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273" s="2" t="s">
         <v>247</v>
       </c>
@@ -13502,7 +13695,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277" s="2" t="s">
         <v>251</v>
       </c>
@@ -13626,7 +13819,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281" s="2" t="s">
         <v>255</v>
       </c>
@@ -13686,7 +13879,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283" s="2" t="s">
         <v>257</v>
       </c>
@@ -13718,7 +13911,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284" s="2" t="s">
         <v>258</v>
       </c>
@@ -13748,7 +13941,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285" s="2" t="s">
         <v>259</v>
       </c>
@@ -13842,7 +14035,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288" s="2" t="s">
         <v>262</v>
       </c>
@@ -13904,7 +14097,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="290" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290" s="2" t="s">
         <v>264</v>
       </c>
@@ -14250,7 +14443,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="301" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301" s="2" t="s">
         <v>275</v>
       </c>
@@ -14314,7 +14507,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="303" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303" s="2" t="s">
         <v>277</v>
       </c>
@@ -14346,7 +14539,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="304" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304" s="2" t="s">
         <v>278</v>
       </c>
@@ -14502,7 +14695,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="309" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309" s="2" t="s">
         <v>283</v>
       </c>
@@ -14566,7 +14759,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="311" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311" s="2" t="s">
         <v>285</v>
       </c>
@@ -14598,7 +14791,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="312" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312" s="2" t="s">
         <v>286</v>
       </c>
@@ -14722,7 +14915,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="316" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A316" s="2" t="s">
         <v>290</v>
       </c>
@@ -14850,7 +15043,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="320" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A320" s="2" t="s">
         <v>294</v>
       </c>
@@ -14976,7 +15169,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="324" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A324" s="2" t="s">
         <v>298</v>
       </c>
@@ -15006,7 +15199,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="325" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A325" s="2" t="s">
         <v>299</v>
       </c>
@@ -15038,7 +15231,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="326" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A326" s="2" t="s">
         <v>300</v>
       </c>
@@ -15070,7 +15263,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="327" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A327" s="2" t="s">
         <v>301</v>
       </c>
@@ -15102,7 +15295,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="328" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A328" s="2" t="s">
         <v>302</v>
       </c>
@@ -15134,7 +15327,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="329" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A329" s="2" t="s">
         <v>303</v>
       </c>
@@ -15198,7 +15391,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="331" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A331" s="2" t="s">
         <v>305</v>
       </c>
@@ -15230,7 +15423,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="332" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A332" s="2" t="s">
         <v>306</v>
       </c>
@@ -15262,7 +15455,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="333" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A333" s="2" t="s">
         <v>307</v>
       </c>
@@ -15294,7 +15487,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="334" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A334" s="2" t="s">
         <v>308</v>
       </c>
@@ -15358,7 +15551,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="336" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A336" s="2" t="s">
         <v>310</v>
       </c>
@@ -15388,7 +15581,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="337" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A337" s="2" t="s">
         <v>311</v>
       </c>
@@ -15420,7 +15613,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="338" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A338" s="2" t="s">
         <v>312</v>
       </c>
@@ -15608,7 +15801,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="344" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A344" s="2" t="s">
         <v>318</v>
       </c>
@@ -15640,7 +15833,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="345" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A345" s="2" t="s">
         <v>319</v>
       </c>
@@ -15672,7 +15865,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="346" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A346" s="2" t="s">
         <v>320</v>
       </c>
@@ -15704,7 +15897,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="347" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A347" s="2" t="s">
         <v>321</v>
       </c>
@@ -15736,7 +15929,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="348" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A348" s="2" t="s">
         <v>322</v>
       </c>
@@ -15766,7 +15959,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="349" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A349" s="2" t="s">
         <v>323</v>
       </c>
@@ -15892,7 +16085,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="353" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A353" s="2" t="s">
         <v>327</v>
       </c>
@@ -16178,7 +16371,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="362" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A362" s="2" t="s">
         <v>336</v>
       </c>
@@ -16208,7 +16401,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="363" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A363" s="2" t="s">
         <v>337</v>
       </c>
@@ -16368,7 +16561,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="368" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A368" s="2" t="s">
         <v>342</v>
       </c>
@@ -16400,7 +16593,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="369" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A369" s="2" t="s">
         <v>343</v>
       </c>
@@ -16590,7 +16783,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="375" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A375" s="2" t="s">
         <v>349</v>
       </c>
@@ -16622,7 +16815,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="376" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A376" s="2" t="s">
         <v>350</v>
       </c>
@@ -16684,7 +16877,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="378" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A378" s="2" t="s">
         <v>352</v>
       </c>
@@ -16812,7 +17005,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="382" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A382" s="2" t="s">
         <v>356</v>
       </c>
@@ -16876,7 +17069,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="384" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A384" s="2" t="s">
         <v>358</v>
       </c>
@@ -16908,7 +17101,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="385" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A385" s="2" t="s">
         <v>359</v>
       </c>
@@ -17004,7 +17197,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="388" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A388" s="2" t="s">
         <v>362</v>
       </c>
@@ -17036,7 +17229,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="389" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A389" s="2" t="s">
         <v>363</v>
       </c>
@@ -17068,7 +17261,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="390" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A390" s="2" t="s">
         <v>364</v>
       </c>
@@ -17164,7 +17357,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="393" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A393" s="2" t="s">
         <v>367</v>
       </c>
@@ -17228,7 +17421,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="395" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A395" s="2" t="s">
         <v>369</v>
       </c>
@@ -17260,7 +17453,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="396" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A396" s="2" t="s">
         <v>370</v>
       </c>
@@ -17290,7 +17483,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="397" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A397" s="2" t="s">
         <v>371</v>
       </c>
@@ -17384,7 +17577,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="400" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A400" s="2" t="s">
         <v>374</v>
       </c>
@@ -17416,7 +17609,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="401" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A401" s="2" t="s">
         <v>375</v>
       </c>
@@ -17480,7 +17673,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="403" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A403" s="2" t="s">
         <v>377</v>
       </c>
@@ -17576,7 +17769,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="406" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A406" s="2" t="s">
         <v>380</v>
       </c>
@@ -17608,7 +17801,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="407" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A407" s="2" t="s">
         <v>381</v>
       </c>
@@ -17670,7 +17863,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="409" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A409" s="2" t="s">
         <v>383</v>
       </c>
@@ -18022,7 +18215,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="420" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A420" s="2" t="s">
         <v>394</v>
       </c>
@@ -18054,7 +18247,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="421" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A421" s="2" t="s">
         <v>395</v>
       </c>
@@ -18086,7 +18279,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="422" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A422" s="2" t="s">
         <v>396</v>
       </c>
@@ -18118,7 +18311,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="423" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A423" s="2" t="s">
         <v>397</v>
       </c>
@@ -18150,7 +18343,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="424" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A424" s="2" t="s">
         <v>398</v>
       </c>
@@ -18180,7 +18373,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="425" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A425" s="2" t="s">
         <v>399</v>
       </c>
@@ -18244,7 +18437,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="427" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A427" s="2" t="s">
         <v>401</v>
       </c>
@@ -18276,7 +18469,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="428" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A428" s="2" t="s">
         <v>402</v>
       </c>
@@ -18340,7 +18533,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="430" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A430" s="2" t="s">
         <v>404</v>
       </c>
@@ -18370,7 +18563,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="431" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A431" s="2" t="s">
         <v>405</v>
       </c>
@@ -18402,7 +18595,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="432" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A432" s="2" t="s">
         <v>406</v>
       </c>
@@ -18496,7 +18689,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="435" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A435" s="2" t="s">
         <v>409</v>
       </c>
@@ -18526,7 +18719,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="436" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A436" s="2" t="s">
         <v>410</v>
       </c>
@@ -18588,7 +18781,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="438" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A438" s="2" t="s">
         <v>412</v>
       </c>
@@ -18780,7 +18973,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="444" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A444" s="2" t="s">
         <v>418</v>
       </c>
@@ -18810,7 +19003,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="445" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A445" s="2" t="s">
         <v>419</v>
       </c>
@@ -18842,7 +19035,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="446" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A446" s="2" t="s">
         <v>420</v>
       </c>
@@ -19030,7 +19223,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="452" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A452" s="2" t="s">
         <v>426</v>
       </c>
@@ -19094,7 +19287,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="454" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A454" s="2" t="s">
         <v>428</v>
       </c>
@@ -19156,7 +19349,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="456" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A456" s="2" t="s">
         <v>430</v>
       </c>
@@ -19250,7 +19443,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="459" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A459" s="2" t="s">
         <v>433</v>
       </c>
@@ -19378,7 +19571,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="463" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A463" s="2" t="s">
         <v>437</v>
       </c>
@@ -19756,7 +19949,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="475" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A475" s="2" t="s">
         <v>449</v>
       </c>
@@ -20042,7 +20235,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="484" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A484" s="2" t="s">
         <v>458</v>
       </c>
@@ -20168,7 +20361,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="488" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A488" s="2" t="s">
         <v>462</v>
       </c>
@@ -20418,7 +20611,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="496" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A496" s="2" t="s">
         <v>470</v>
       </c>
@@ -20482,7 +20675,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="498" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A498" s="2" t="s">
         <v>472</v>
       </c>
@@ -20862,7 +21055,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="510" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="510" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A510" s="2" t="s">
         <v>484</v>
       </c>
@@ -21086,7 +21279,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="517" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="517" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A517" s="2" t="s">
         <v>491</v>
       </c>
@@ -21244,7 +21437,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="522" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="522" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A522" s="2" t="s">
         <v>496</v>
       </c>
@@ -22030,7 +22223,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="547" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="547" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A547" s="2" t="s">
         <v>521</v>
       </c>
@@ -22284,7 +22477,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="555" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="555" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A555" s="2" t="s">
         <v>529</v>
       </c>
@@ -22314,7 +22507,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="556" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="556" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A556" s="2" t="s">
         <v>530</v>
       </c>
@@ -22438,7 +22631,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="560" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="560" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A560" s="2" t="s">
         <v>534</v>
       </c>
@@ -22468,7 +22661,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="561" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="561" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A561" s="2" t="s">
         <v>535</v>
       </c>
@@ -22780,7 +22973,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="571" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="571" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A571" s="2" t="s">
         <v>545</v>
       </c>
@@ -22964,7 +23157,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="577" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="577" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A577" s="2" t="s">
         <v>551</v>
       </c>
@@ -23152,7 +23345,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="583" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="583" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A583" s="2" t="s">
         <v>557</v>
       </c>
@@ -23184,7 +23377,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="584" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="584" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A584" s="2" t="s">
         <v>558</v>
       </c>
@@ -23338,7 +23531,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="589" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="589" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A589" s="2" t="s">
         <v>563</v>
       </c>
@@ -23432,7 +23625,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="592" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="592" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A592" s="2" t="s">
         <v>566</v>
       </c>
@@ -23588,7 +23781,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="597" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="597" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A597" s="2" t="s">
         <v>571</v>
       </c>
@@ -23896,7 +24089,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="607" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="607" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A607" s="2" t="s">
         <v>581</v>
       </c>
@@ -24054,7 +24247,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="612" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="612" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A612" s="2" t="s">
         <v>586</v>
       </c>
@@ -24276,7 +24469,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="619" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="619" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A619" s="2" t="s">
         <v>593</v>
       </c>
@@ -24308,7 +24501,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="620" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="620" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A620" s="2" t="s">
         <v>594</v>
       </c>
@@ -24338,7 +24531,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="621" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="621" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A621" s="2" t="s">
         <v>595</v>
       </c>
@@ -24588,7 +24781,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="629" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="629" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A629" s="2" t="s">
         <v>603</v>
       </c>
@@ -24778,7 +24971,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="635" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="635" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A635" s="2" t="s">
         <v>609</v>
       </c>
@@ -24840,7 +25033,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="637" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="637" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A637" s="2" t="s">
         <v>611</v>
       </c>
@@ -25028,7 +25221,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="643" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="643" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A643" s="2" t="s">
         <v>617</v>
       </c>
@@ -25344,7 +25537,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="653" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="653" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A653" s="2" t="s">
         <v>627</v>
       </c>
@@ -25628,7 +25821,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="662" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="662" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A662" s="2" t="s">
         <v>636</v>
       </c>
@@ -25660,7 +25853,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="663" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="663" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A663" s="2" t="s">
         <v>637</v>
       </c>
@@ -25690,7 +25883,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="664" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="664" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A664" s="2" t="s">
         <v>638</v>
       </c>
@@ -25720,7 +25913,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="665" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="665" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A665" s="2" t="s">
         <v>639</v>
       </c>
@@ -25752,7 +25945,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="666" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="666" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A666" s="2" t="s">
         <v>640</v>
       </c>
@@ -25908,7 +26101,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="671" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="671" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A671" s="2" t="s">
         <v>645</v>
       </c>
@@ -26222,7 +26415,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="681" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="681" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A681" s="2" t="s">
         <v>655</v>
       </c>
@@ -26380,7 +26573,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="686" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="686" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A686" s="2" t="s">
         <v>660</v>
       </c>
@@ -26444,7 +26637,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="688" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="688" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A688" s="2" t="s">
         <v>662</v>
       </c>
@@ -26476,7 +26669,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="689" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="689" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A689" s="2" t="s">
         <v>663</v>
       </c>
@@ -26508,7 +26701,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="690" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="690" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A690" s="2" t="s">
         <v>664</v>
       </c>
@@ -26540,7 +26733,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="691" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="691" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A691" s="2" t="s">
         <v>665</v>
       </c>
@@ -26570,7 +26763,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="692" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="692" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A692" s="2" t="s">
         <v>666</v>
       </c>
@@ -26600,7 +26793,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="693" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="693" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A693" s="2" t="s">
         <v>667</v>
       </c>
@@ -26786,7 +26979,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="699" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="699" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A699" s="2" t="s">
         <v>673</v>
       </c>
@@ -26848,7 +27041,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="701" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="701" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A701" s="2" t="s">
         <v>675</v>
       </c>
@@ -26944,7 +27137,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="704" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="704" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A704" s="2" t="s">
         <v>678</v>
       </c>
@@ -27196,7 +27389,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="712" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="712" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A712" s="2" t="s">
         <v>686</v>
       </c>
@@ -27226,7 +27419,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="713" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="713" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A713" s="2" t="s">
         <v>687</v>
       </c>
@@ -27414,7 +27607,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="719" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="719" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A719" s="2" t="s">
         <v>693</v>
       </c>
@@ -27446,7 +27639,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="720" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="720" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A720" s="2" t="s">
         <v>694</v>
       </c>
@@ -27476,7 +27669,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="721" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="721" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A721" s="2" t="s">
         <v>695</v>
       </c>
@@ -27540,7 +27733,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="723" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="723" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A723" s="2" t="s">
         <v>697</v>
       </c>
@@ -27572,7 +27765,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="724" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="724" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A724" s="2" t="s">
         <v>698</v>
       </c>
@@ -27700,7 +27893,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="728" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="728" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A728" s="2" t="s">
         <v>702</v>
       </c>
@@ -27860,7 +28053,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="733" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="733" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A733" s="2" t="s">
         <v>707</v>
       </c>
@@ -27954,7 +28147,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="736" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="736" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A736" s="2" t="s">
         <v>710</v>
       </c>
@@ -28016,7 +28209,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="738" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="738" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A738" s="2" t="s">
         <v>712</v>
       </c>
@@ -28048,7 +28241,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="739" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="739" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A739" s="2" t="s">
         <v>713</v>
       </c>
@@ -28080,7 +28273,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="740" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="740" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A740" s="2" t="s">
         <v>714</v>
       </c>
@@ -28268,7 +28461,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="746" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="746" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A746" s="2" t="s">
         <v>720</v>
       </c>
@@ -28392,7 +28585,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="750" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="750" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A750" s="2" t="s">
         <v>724</v>
       </c>
@@ -28456,7 +28649,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="752" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="752" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A752" s="2" t="s">
         <v>726</v>
       </c>
@@ -28488,7 +28681,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="753" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="753" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A753" s="2" t="s">
         <v>727</v>
       </c>
@@ -28520,7 +28713,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="754" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="754" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A754" s="2" t="s">
         <v>728</v>
       </c>
@@ -28552,7 +28745,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="755" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="755" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A755" s="2" t="s">
         <v>729</v>
       </c>
@@ -28836,7 +29029,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="764" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="764" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A764" s="2" t="s">
         <v>738</v>
       </c>
@@ -28900,7 +29093,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="766" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="766" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A766" s="2" t="s">
         <v>740</v>
       </c>
@@ -28932,7 +29125,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="767" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="767" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A767" s="2" t="s">
         <v>741</v>
       </c>
@@ -28962,7 +29155,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="768" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="768" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A768" s="2" t="s">
         <v>742</v>
       </c>
@@ -29090,7 +29283,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="772" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="772" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A772" s="2" t="s">
         <v>746</v>
       </c>
@@ -29154,7 +29347,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="774" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="774" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A774" s="2" t="s">
         <v>748</v>
       </c>
@@ -29218,7 +29411,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="776" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="776" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A776" s="2" t="s">
         <v>750</v>
       </c>
@@ -29346,7 +29539,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="780" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="780" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A780" s="2" t="s">
         <v>754</v>
       </c>
@@ -29570,7 +29763,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="787" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="787" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A787" s="2" t="s">
         <v>761</v>
       </c>
@@ -29858,7 +30051,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="796" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="796" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A796" s="2" t="s">
         <v>770</v>
       </c>
@@ -30082,7 +30275,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="803" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="803" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A803" s="2" t="s">
         <v>777</v>
       </c>
@@ -30206,7 +30399,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="807" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="807" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A807" s="2" t="s">
         <v>781</v>
       </c>
@@ -30266,7 +30459,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="809" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="809" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A809" s="2" t="s">
         <v>783</v>
       </c>
@@ -30642,7 +30835,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="821" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="821" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A821" s="2" t="s">
         <v>795</v>
       </c>
@@ -30674,7 +30867,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="822" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="822" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A822" s="2" t="s">
         <v>796</v>
       </c>
@@ -30926,7 +31119,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="830" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="830" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A830" s="2" t="s">
         <v>804</v>
       </c>
@@ -30954,7 +31147,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="831" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="831" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A831" s="2" t="s">
         <v>805</v>
       </c>
@@ -30984,7 +31177,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="832" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="832" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A832" s="2" t="s">
         <v>806</v>
       </c>
@@ -31016,7 +31209,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="833" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="833" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A833" s="2" t="s">
         <v>807</v>
       </c>
@@ -31080,7 +31273,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="835" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="835" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A835" s="2" t="s">
         <v>809</v>
       </c>
@@ -33282,7 +33475,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="905" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="905" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A905" s="2" t="s">
         <v>879</v>
       </c>
@@ -33506,7 +33699,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="912" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="912" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A912" s="2" t="s">
         <v>886</v>
       </c>
@@ -33792,7 +33985,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="921" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="921" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A921" s="2" t="s">
         <v>895</v>
       </c>
@@ -33980,7 +34173,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="927" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="927" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A927" s="2" t="s">
         <v>901</v>
       </c>
@@ -34422,7 +34615,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="941" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="941" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A941" s="2" t="s">
         <v>915</v>
       </c>
@@ -34454,7 +34647,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="942" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="942" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A942" s="2" t="s">
         <v>916</v>
       </c>
@@ -34516,7 +34709,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="944" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="944" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A944" s="2" t="s">
         <v>918</v>
       </c>
@@ -34546,7 +34739,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="945" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="945" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A945" s="2" t="s">
         <v>919</v>
       </c>
@@ -34672,7 +34865,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="949" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="949" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A949" s="2" t="s">
         <v>923</v>
       </c>
@@ -34736,7 +34929,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="951" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="951" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A951" s="2" t="s">
         <v>925</v>
       </c>
@@ -34830,7 +35023,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="954" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="954" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A954" s="2" t="s">
         <v>928</v>
       </c>
@@ -34924,7 +35117,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="957" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="957" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A957" s="2" t="s">
         <v>931</v>
       </c>
@@ -35048,7 +35241,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="961" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="961" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A961" s="2" t="s">
         <v>935</v>
       </c>
@@ -35080,7 +35273,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="962" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="962" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A962" s="2" t="s">
         <v>936</v>
       </c>
@@ -35174,7 +35367,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="965" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="965" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A965" s="2" t="s">
         <v>939</v>
       </c>
@@ -35206,7 +35399,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="966" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="966" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A966" s="2" t="s">
         <v>940</v>
       </c>
@@ -35426,7 +35619,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="973" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="973" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A973" s="2" t="s">
         <v>947</v>
       </c>
@@ -36494,7 +36687,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1007" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1007" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1007" s="2" t="s">
         <v>1395</v>
       </c>
@@ -36806,7 +36999,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1017" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1017" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1017" s="2" t="s">
         <v>960</v>
       </c>
@@ -36838,7 +37031,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1018" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1018" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1018" s="2" t="s">
         <v>961</v>
       </c>
@@ -36932,7 +37125,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1021" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1021" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1021" s="2" t="s">
         <v>964</v>
       </c>
@@ -36964,7 +37157,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1022" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1022" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1022" s="2" t="s">
         <v>965</v>
       </c>
@@ -37026,7 +37219,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1024" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1024" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1024" s="2" t="s">
         <v>967</v>
       </c>
@@ -37118,7 +37311,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1027" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1027" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1027" s="2" t="s">
         <v>970</v>
       </c>
@@ -37577,7 +37770,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1042" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1042" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1042" s="2" t="s">
         <v>985</v>
       </c>
@@ -37861,7 +38054,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1051" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1051" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1051" s="2" t="s">
         <v>1407</v>
       </c>
@@ -38019,7 +38212,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1056" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1056" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1056" s="2" t="s">
         <v>1412</v>
       </c>
@@ -38051,7 +38244,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1057" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1057" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1057" s="2" t="s">
         <v>1413</v>
       </c>
@@ -38649,7 +38842,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1076" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1076" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1076" s="2" t="s">
         <v>1432</v>
       </c>
@@ -38713,7 +38906,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1078" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1078" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1078" s="2" t="s">
         <v>990</v>
       </c>
@@ -38745,7 +38938,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1079" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1079" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1079" s="2" t="s">
         <v>991</v>
       </c>
@@ -38807,7 +39000,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1081" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1081" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1081" s="2" t="s">
         <v>993</v>
       </c>
@@ -38839,7 +39032,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1082" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1082" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1082" s="2" t="s">
         <v>994</v>
       </c>
@@ -38903,7 +39096,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1084" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1084" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1084" s="2" t="s">
         <v>996</v>
       </c>
@@ -38961,7 +39154,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1086" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1086" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1086" s="2" t="s">
         <v>998</v>
       </c>
@@ -39559,7 +39752,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1105" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1105" s="2" t="s">
         <v>1017</v>
       </c>
@@ -39589,7 +39782,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1106" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1106" s="2" t="s">
         <v>1018</v>
       </c>
@@ -39651,7 +39844,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1108" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1108" s="2" t="s">
         <v>1020</v>
       </c>
@@ -39715,7 +39908,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1110" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1110" s="2" t="s">
         <v>1022</v>
       </c>
@@ -39747,7 +39940,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1111" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1111" s="2" t="s">
         <v>1023</v>
       </c>
@@ -39777,7 +39970,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1112" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1112" s="2" t="s">
         <v>1024</v>
       </c>
@@ -39839,7 +40032,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1114" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1114" s="2" t="s">
         <v>1026</v>
       </c>
@@ -39871,7 +40064,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1115" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1115" s="2" t="s">
         <v>1027</v>
       </c>
@@ -39903,7 +40096,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1116" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1116" s="2" t="s">
         <v>1028</v>
       </c>
@@ -39935,7 +40128,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1117" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1117" s="2" t="s">
         <v>1029</v>
       </c>
@@ -39965,7 +40158,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1118" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1118" s="2" t="s">
         <v>1030</v>
       </c>
@@ -40027,7 +40220,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1120" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1120" s="2" t="s">
         <v>1032</v>
       </c>
@@ -40089,7 +40282,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1122" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1122" s="2" t="s">
         <v>1034</v>
       </c>
@@ -40345,7 +40538,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1130" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1130" s="2" t="s">
         <v>1042</v>
       </c>
@@ -40503,7 +40696,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1135" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1135" s="2" t="s">
         <v>1047</v>
       </c>
@@ -40533,7 +40726,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1136" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1136" s="2" t="s">
         <v>1048</v>
       </c>
@@ -40595,7 +40788,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1138" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1138" s="2" t="s">
         <v>1050</v>
       </c>
@@ -40627,7 +40820,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1139" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1139" s="2" t="s">
         <v>1051</v>
       </c>
@@ -40659,7 +40852,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1140" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1140" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1140" s="2" t="s">
         <v>1052</v>
       </c>
@@ -40755,7 +40948,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1143" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1143" s="2" t="s">
         <v>1055</v>
       </c>
@@ -40819,7 +41012,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1145" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1145" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1145" s="2" t="s">
         <v>1057</v>
       </c>
@@ -40851,7 +41044,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1146" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1146" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1146" s="2" t="s">
         <v>1058</v>
       </c>
@@ -40883,7 +41076,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1147" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1147" s="2" t="s">
         <v>1059</v>
       </c>
@@ -40945,7 +41138,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1149" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1149" s="2" t="s">
         <v>1061</v>
       </c>
@@ -40977,7 +41170,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1150" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1150" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1150" s="2" t="s">
         <v>1062</v>
       </c>
@@ -41009,7 +41202,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1151" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1151" s="2" t="s">
         <v>1063</v>
       </c>
@@ -41039,7 +41232,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1152" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1152" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1152" s="2" t="s">
         <v>1064</v>
       </c>
@@ -41199,7 +41392,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1157" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1157" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1157" s="2" t="s">
         <v>1069</v>
       </c>
@@ -41261,7 +41454,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1159" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1159" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1159" s="2" t="s">
         <v>1071</v>
       </c>
@@ -41293,7 +41486,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1160" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1160" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1160" s="2" t="s">
         <v>1072</v>
       </c>
@@ -41325,7 +41518,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1161" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1161" s="2" t="s">
         <v>1073</v>
       </c>
@@ -41357,7 +41550,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1162" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1162" s="2" t="s">
         <v>1074</v>
       </c>
@@ -41579,7 +41772,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1169" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1169" s="2" t="s">
         <v>1081</v>
       </c>
@@ -41707,7 +41900,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1173" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1173" s="2" t="s">
         <v>1085</v>
       </c>
@@ -41739,7 +41932,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1174" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1174" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1174" s="2" t="s">
         <v>1086</v>
       </c>
@@ -41803,7 +41996,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1176" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1176" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1176" s="2" t="s">
         <v>1088</v>
       </c>
@@ -41833,7 +42026,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1177" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1177" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1177" s="2" t="s">
         <v>1089</v>
       </c>
@@ -42237,7 +42430,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1190" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1190" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1190" s="2" t="s">
         <v>1102</v>
       </c>
@@ -42363,7 +42556,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1194" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1194" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1194" s="2" t="s">
         <v>1106</v>
       </c>
@@ -42393,7 +42586,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1195" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1195" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1195" s="2" t="s">
         <v>1107</v>
       </c>
@@ -42485,7 +42678,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1198" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1198" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1198" s="2" t="s">
         <v>1110</v>
       </c>
@@ -42549,7 +42742,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1200" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1200" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1200" s="2" t="s">
         <v>1112</v>
       </c>
@@ -42675,7 +42868,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1204" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1204" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1204" s="2" t="s">
         <v>1116</v>
       </c>
@@ -42705,7 +42898,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1205" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1205" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1205" s="2" t="s">
         <v>1117</v>
       </c>
@@ -43051,7 +43244,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1216" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1216" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1216" s="2" t="s">
         <v>1128</v>
       </c>
@@ -43173,7 +43366,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1220" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1220" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1220" s="2" t="s">
         <v>1132</v>
       </c>
@@ -43419,7 +43612,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1228" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1228" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1228" s="2" t="s">
         <v>1140</v>
       </c>
@@ -43449,7 +43642,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1229" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1229" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1229" s="2" t="s">
         <v>1141</v>
       </c>
@@ -43757,7 +43950,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1239" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1239" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1239" s="2" t="s">
         <v>1151</v>
       </c>
@@ -43945,7 +44138,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1245" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1245" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1245" s="2" t="s">
         <v>1157</v>
       </c>
@@ -44251,7 +44444,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1255" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1255" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1255" s="2" t="s">
         <v>1167</v>
       </c>
@@ -44281,7 +44474,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1256" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1256" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1256" s="2" t="s">
         <v>1168</v>
       </c>
@@ -44469,7 +44662,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1262" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1262" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1262" s="2" t="s">
         <v>1174</v>
       </c>
@@ -44501,7 +44694,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1263" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1263" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1263" s="2" t="s">
         <v>1175</v>
       </c>
@@ -44563,7 +44756,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1265" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1265" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1265" s="2" t="s">
         <v>1177</v>
       </c>
@@ -44595,7 +44788,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1266" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1266" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1266" s="2" t="s">
         <v>1178</v>
       </c>
@@ -44963,7 +45156,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1278" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1278" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1278" s="2" t="s">
         <v>1190</v>
       </c>
@@ -45337,7 +45530,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1290" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1290" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1290" s="2" t="s">
         <v>1202</v>
       </c>
@@ -45497,7 +45690,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1295" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1295" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1295" s="2" t="s">
         <v>1207</v>
       </c>
@@ -45529,7 +45722,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1296" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1296" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1296" s="2" t="s">
         <v>1208</v>
       </c>
@@ -45593,7 +45786,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1298" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1298" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1298" s="2" t="s">
         <v>1210</v>
       </c>
@@ -45689,7 +45882,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1301" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1301" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1301" s="2" t="s">
         <v>1213</v>
       </c>
@@ -45977,7 +46170,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1310" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1310" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1310" s="2" t="s">
         <v>1222</v>
       </c>
@@ -46105,7 +46298,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1314" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1314" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1314" s="2" t="s">
         <v>1226</v>
       </c>
@@ -46297,7 +46490,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1320" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1320" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1320" s="2" t="s">
         <v>1232</v>
       </c>
@@ -46777,7 +46970,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1335" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1335" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1335" s="2" t="s">
         <v>1247</v>
       </c>
@@ -46841,7 +47034,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1337" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1337" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1337" s="2" t="s">
         <v>1249</v>
       </c>
@@ -47033,7 +47226,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1343" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1343" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1343" s="2" t="s">
         <v>1255</v>
       </c>
@@ -47161,7 +47354,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1347" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1347" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1347" s="2" t="s">
         <v>1259</v>
       </c>
@@ -47193,7 +47386,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1348" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1348" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1348" s="2" t="s">
         <v>1260</v>
       </c>
@@ -47225,7 +47418,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1349" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1349" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1349" s="2" t="s">
         <v>1261</v>
       </c>
@@ -47321,7 +47514,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1352" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1352" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1352" s="2" t="s">
         <v>1264</v>
       </c>
@@ -47449,7 +47642,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1356" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1356" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1356" s="2" t="s">
         <v>1268</v>
       </c>
@@ -47481,7 +47674,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1357" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1357" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1357" s="2" t="s">
         <v>1269</v>
       </c>
@@ -47513,7 +47706,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1358" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1358" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1358" s="2" t="s">
         <v>1270</v>
       </c>
@@ -47609,7 +47802,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1361" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1361" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1361" s="2" t="s">
         <v>1273</v>
       </c>
@@ -47833,7 +48026,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1368" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1368" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1368" s="2" t="s">
         <v>1280</v>
       </c>
@@ -48057,7 +48250,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1375" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1375" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1375" s="2" t="s">
         <v>1287</v>
       </c>
@@ -48537,7 +48730,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1390" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1390" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1390" s="2" t="s">
         <v>1302</v>
       </c>
@@ -48761,7 +48954,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1397" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1397" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1397" s="2" t="s">
         <v>1309</v>
       </c>
@@ -48953,7 +49146,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1403" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1403" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1403" s="2" t="s">
         <v>1315</v>
       </c>
@@ -49049,7 +49242,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1406" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1406" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1406" s="2" t="s">
         <v>1318</v>
       </c>
@@ -49465,7 +49658,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1419" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1419" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1419" s="2" t="s">
         <v>1331</v>
       </c>
@@ -49593,7 +49786,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1423" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1423" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1423" s="2" t="s">
         <v>1335</v>
       </c>
@@ -49689,7 +49882,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1426" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1426" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1426" s="2" t="s">
         <v>1338</v>
       </c>
@@ -49785,7 +49978,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1429" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1429" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1429" s="2" t="s">
         <v>1433</v>
       </c>
@@ -49817,7 +50010,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1430" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1430" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1430" s="2" t="s">
         <v>1434</v>
       </c>
@@ -49849,7 +50042,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1431" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1431" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1431" s="2" t="s">
         <v>1435</v>
       </c>
@@ -49881,7 +50074,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1432" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1432" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1432" s="2" t="s">
         <v>1436</v>
       </c>
@@ -49913,7 +50106,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1433" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1433" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1433" s="2" t="s">
         <v>1437</v>
       </c>
@@ -49945,7 +50138,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1434" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1434" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1434" s="2" t="s">
         <v>1438</v>
       </c>
@@ -49977,7 +50170,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1435" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1435" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1435" s="2" t="s">
         <v>1439</v>
       </c>
@@ -50169,7 +50362,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1441" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1441" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1441" s="2" t="s">
         <v>1445</v>
       </c>
@@ -50202,11 +50395,687 @@
       </c>
     </row>
     <row r="1442" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1442" s="8"/>
-      <c r="G1442" s="1"/>
+      <c r="A1442" s="1" t="s">
+        <v>1463</v>
+      </c>
+      <c r="B1442" s="1">
+        <v>29.7</v>
+      </c>
+      <c r="C1442" s="1">
+        <v>71</v>
+      </c>
+      <c r="D1442" s="1">
+        <v>1</v>
+      </c>
+      <c r="E1442" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="F1442" s="1">
+        <v>1</v>
+      </c>
+      <c r="G1442" s="1" t="s">
+        <v>1458</v>
+      </c>
+      <c r="H1442" s="6" t="s">
+        <v>1485</v>
+      </c>
+      <c r="I1442" s="6" t="s">
+        <v>1486</v>
+      </c>
+      <c r="J1442" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1443" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A1443" s="1" t="s">
+        <v>1464</v>
+      </c>
+      <c r="B1443" s="1">
+        <v>29.7</v>
+      </c>
+      <c r="C1443" s="1">
+        <v>69</v>
+      </c>
+      <c r="D1443" s="1">
+        <v>1</v>
+      </c>
+      <c r="E1443" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="F1443" s="1">
+        <v>2</v>
+      </c>
+      <c r="G1443" s="1" t="s">
+        <v>1461</v>
+      </c>
+      <c r="H1443" s="6" t="s">
+        <v>1487</v>
+      </c>
+      <c r="I1443" s="6" t="s">
+        <v>1488</v>
+      </c>
+      <c r="J1443" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1444" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1444" s="1" t="s">
+        <v>1465</v>
+      </c>
+      <c r="B1444" s="1">
+        <v>30.1</v>
+      </c>
+      <c r="C1444" s="1">
+        <v>68</v>
+      </c>
+      <c r="D1444" s="1" t="s">
+        <v>1466</v>
+      </c>
+      <c r="E1444" s="1">
+        <v>4</v>
+      </c>
+      <c r="F1444" s="1">
+        <v>1</v>
+      </c>
+      <c r="G1444" s="1" t="s">
+        <v>1458</v>
+      </c>
+      <c r="H1444" s="6" t="s">
+        <v>1489</v>
+      </c>
+      <c r="I1444" s="6" t="s">
+        <v>1490</v>
+      </c>
+      <c r="J1444" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1445" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A1445" s="1" t="s">
+        <v>1467</v>
+      </c>
+      <c r="B1445" s="1">
+        <v>28.4</v>
+      </c>
+      <c r="C1445" s="1">
+        <v>75</v>
+      </c>
+      <c r="D1445" s="1" t="s">
+        <v>1466</v>
+      </c>
+      <c r="E1445" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="F1445" s="1">
+        <v>2</v>
+      </c>
+      <c r="G1445" s="1" t="s">
+        <v>1461</v>
+      </c>
+      <c r="H1445" s="6" t="s">
+        <v>1491</v>
+      </c>
+      <c r="I1445" s="6" t="s">
+        <v>1492</v>
+      </c>
+      <c r="J1445" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1446" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1446" s="1" t="s">
+        <v>1468</v>
+      </c>
+      <c r="B1446" s="1">
+        <v>28.3</v>
+      </c>
+      <c r="C1446" s="1">
+        <v>78</v>
+      </c>
+      <c r="D1446" s="1" t="s">
+        <v>1466</v>
+      </c>
+      <c r="E1446" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="F1446" s="1">
+        <v>1</v>
+      </c>
+      <c r="G1446" s="1" t="s">
+        <v>1458</v>
+      </c>
+      <c r="H1446" s="6" t="s">
+        <v>1493</v>
+      </c>
+      <c r="I1446" s="6" t="s">
+        <v>1494</v>
+      </c>
+      <c r="J1446" s="7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1447" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1447" s="1" t="s">
+        <v>1469</v>
+      </c>
+      <c r="B1447" s="1">
+        <v>28.4</v>
+      </c>
+      <c r="C1447" s="1">
+        <v>79</v>
+      </c>
+      <c r="D1447" s="1">
+        <v>19</v>
+      </c>
+      <c r="E1447" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="F1447" s="1">
+        <v>1</v>
+      </c>
+      <c r="G1447" s="1" t="s">
+        <v>1458</v>
+      </c>
+      <c r="H1447" s="6" t="s">
+        <v>1495</v>
+      </c>
+      <c r="I1447" s="6" t="s">
+        <v>1496</v>
+      </c>
+      <c r="J1447" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1448" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1448" s="1" t="s">
+        <v>1470</v>
+      </c>
+      <c r="B1448" s="1">
+        <v>28.3</v>
+      </c>
+      <c r="C1448" s="1">
+        <v>82</v>
+      </c>
+      <c r="D1448" s="1">
+        <v>7</v>
+      </c>
+      <c r="E1448" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F1448" s="1">
+        <v>1</v>
+      </c>
+      <c r="G1448" s="1" t="s">
+        <v>1458</v>
+      </c>
+      <c r="H1448" s="6" t="s">
+        <v>1497</v>
+      </c>
+      <c r="I1448" s="6" t="s">
+        <v>1498</v>
+      </c>
+      <c r="J1448" s="7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1449" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A1449" s="1" t="s">
+        <v>1471</v>
+      </c>
+      <c r="B1449" s="1">
+        <v>29.1</v>
+      </c>
+      <c r="C1449" s="1">
+        <v>72</v>
+      </c>
+      <c r="D1449" s="1">
+        <v>8888</v>
+      </c>
+      <c r="E1449" s="1">
+        <v>2</v>
+      </c>
+      <c r="F1449" s="1">
+        <v>2</v>
+      </c>
+      <c r="G1449" s="1" t="s">
+        <v>1461</v>
+      </c>
+      <c r="H1449" s="6" t="s">
+        <v>1499</v>
+      </c>
+      <c r="I1449" s="6" t="s">
+        <v>1500</v>
+      </c>
+      <c r="J1449" s="7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1450" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1450" s="1" t="s">
+        <v>1472</v>
+      </c>
+      <c r="B1450" s="1">
+        <v>28.1</v>
+      </c>
+      <c r="C1450" s="1">
+        <v>82</v>
+      </c>
+      <c r="D1450" s="1">
+        <v>1</v>
+      </c>
+      <c r="E1450" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="F1450" s="1">
+        <v>1</v>
+      </c>
+      <c r="G1450" s="1" t="s">
+        <v>1458</v>
+      </c>
+      <c r="H1450" s="6" t="s">
+        <v>1501</v>
+      </c>
+      <c r="I1450" s="6" t="s">
+        <v>1502</v>
+      </c>
+      <c r="J1450" s="7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1451" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1451" s="1" t="s">
+        <v>1473</v>
+      </c>
+      <c r="B1451" s="1">
+        <v>28.1</v>
+      </c>
+      <c r="C1451" s="1">
+        <v>82</v>
+      </c>
+      <c r="D1451" s="1">
+        <v>56</v>
+      </c>
+      <c r="E1451" s="1">
+        <v>1.9</v>
+      </c>
+      <c r="F1451" s="1">
+        <v>1</v>
+      </c>
+      <c r="G1451" s="1" t="s">
+        <v>1458</v>
+      </c>
+      <c r="H1451" s="6" t="s">
+        <v>1503</v>
+      </c>
+      <c r="I1451" s="6" t="s">
+        <v>1504</v>
+      </c>
+      <c r="J1451" s="7">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1452" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A1452" s="1" t="s">
+        <v>1474</v>
+      </c>
+      <c r="B1452" s="1">
+        <v>28.1</v>
+      </c>
+      <c r="C1452" s="1">
+        <v>81</v>
+      </c>
+      <c r="D1452" s="1">
+        <v>10</v>
+      </c>
+      <c r="E1452" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="F1452" s="1">
+        <v>2</v>
+      </c>
+      <c r="G1452" s="1" t="s">
+        <v>1458</v>
+      </c>
+      <c r="H1452" s="6" t="s">
+        <v>1505</v>
+      </c>
+      <c r="I1452" s="6" t="s">
+        <v>1506</v>
+      </c>
+      <c r="J1452" s="7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1453" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1453" s="1" t="s">
+        <v>1475</v>
+      </c>
+      <c r="B1453" s="1">
+        <v>27.8</v>
+      </c>
+      <c r="C1453" s="1">
+        <v>87</v>
+      </c>
+      <c r="D1453" s="1">
+        <v>19</v>
+      </c>
+      <c r="E1453" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="F1453" s="1">
+        <v>1</v>
+      </c>
+      <c r="G1453" s="1" t="s">
+        <v>1458</v>
+      </c>
+      <c r="H1453" s="6" t="s">
+        <v>1507</v>
+      </c>
+      <c r="I1453" s="6" t="s">
+        <v>1508</v>
+      </c>
+      <c r="J1453" s="7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1454" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1454" s="1" t="s">
+        <v>1476</v>
+      </c>
+      <c r="B1454" s="1">
+        <v>26.9</v>
+      </c>
+      <c r="C1454" s="1">
+        <v>93</v>
+      </c>
+      <c r="D1454" s="1">
+        <v>44</v>
+      </c>
+      <c r="E1454" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F1454" s="1">
+        <v>1</v>
+      </c>
+      <c r="G1454" s="1" t="s">
+        <v>1458</v>
+      </c>
+      <c r="H1454" s="6" t="s">
+        <v>1509</v>
+      </c>
+      <c r="I1454" s="6" t="s">
+        <v>1510</v>
+      </c>
+      <c r="J1454" s="7">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1455" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1455" s="1" t="s">
+        <v>1477</v>
+      </c>
+      <c r="B1455" s="1">
+        <v>28</v>
+      </c>
+      <c r="C1455" s="1">
+        <v>79</v>
+      </c>
+      <c r="D1455" s="1">
+        <v>17</v>
+      </c>
+      <c r="E1455" s="1" t="s">
+        <v>1466</v>
+      </c>
+      <c r="F1455" s="1">
+        <v>1</v>
+      </c>
+      <c r="G1455" s="1" t="s">
+        <v>1458</v>
+      </c>
+      <c r="H1455" s="6" t="s">
+        <v>1511</v>
+      </c>
+      <c r="I1455" s="6" t="s">
+        <v>1512</v>
+      </c>
+      <c r="J1455" s="7">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1456" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1456" s="1" t="s">
+        <v>1478</v>
+      </c>
+      <c r="B1456" s="1">
+        <v>27.9</v>
+      </c>
+      <c r="C1456" s="1">
+        <v>86</v>
+      </c>
+      <c r="D1456" s="1">
+        <v>3</v>
+      </c>
+      <c r="E1456" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="F1456" s="1">
+        <v>1</v>
+      </c>
+      <c r="G1456" s="1" t="s">
+        <v>1458</v>
+      </c>
+      <c r="H1456" s="6" t="s">
+        <v>1513</v>
+      </c>
+      <c r="I1456" s="6" t="s">
+        <v>1514</v>
+      </c>
+      <c r="J1456" s="7">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1457" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1457" s="1" t="s">
+        <v>1479</v>
+      </c>
+      <c r="B1457" s="1">
+        <v>29.4</v>
+      </c>
+      <c r="C1457" s="1">
+        <v>74</v>
+      </c>
+      <c r="D1457" s="1">
+        <v>8</v>
+      </c>
+      <c r="E1457" s="1" t="s">
+        <v>1466</v>
+      </c>
+      <c r="F1457" s="1">
+        <v>1</v>
+      </c>
+      <c r="G1457" s="1" t="s">
+        <v>1458</v>
+      </c>
+      <c r="H1457" s="6" t="s">
+        <v>1515</v>
+      </c>
+      <c r="I1457" s="6" t="s">
+        <v>1516</v>
+      </c>
+      <c r="J1457" s="7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1458" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A1458" s="1" t="s">
+        <v>1480</v>
+      </c>
+      <c r="B1458" s="1">
+        <v>29.2</v>
+      </c>
+      <c r="C1458" s="1">
+        <v>78</v>
+      </c>
+      <c r="D1458" s="1" t="s">
+        <v>1466</v>
+      </c>
+      <c r="E1458" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="F1458" s="1">
+        <v>2</v>
+      </c>
+      <c r="G1458" s="1" t="s">
+        <v>1458</v>
+      </c>
+      <c r="H1458" s="6" t="s">
+        <v>1517</v>
+      </c>
+      <c r="I1458" s="6" t="s">
+        <v>1518</v>
+      </c>
+      <c r="J1458" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1459" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A1459" s="1" t="s">
+        <v>1481</v>
+      </c>
+      <c r="B1459" s="1">
+        <v>30</v>
+      </c>
+      <c r="C1459" s="1">
+        <v>70</v>
+      </c>
+      <c r="D1459" s="1" t="s">
+        <v>1466</v>
+      </c>
+      <c r="E1459" s="1">
+        <v>3.8</v>
+      </c>
+      <c r="F1459" s="1">
+        <v>2</v>
+      </c>
+      <c r="G1459" s="1" t="s">
+        <v>1458</v>
+      </c>
+      <c r="H1459" s="6" t="s">
+        <v>1519</v>
+      </c>
+      <c r="I1459" s="6" t="s">
+        <v>1520</v>
+      </c>
+      <c r="J1459" s="7">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1460" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1460" s="1" t="s">
+        <v>1482</v>
+      </c>
+      <c r="B1460" s="1">
+        <v>29.7</v>
+      </c>
+      <c r="C1460" s="1">
+        <v>73</v>
+      </c>
+      <c r="D1460" s="1" t="s">
+        <v>1466</v>
+      </c>
+      <c r="E1460" s="1">
+        <v>3</v>
+      </c>
+      <c r="F1460" s="1">
+        <v>1</v>
+      </c>
+      <c r="G1460" s="1" t="s">
+        <v>1458</v>
+      </c>
+      <c r="H1460" s="6" t="s">
+        <v>1521</v>
+      </c>
+      <c r="I1460" s="6" t="s">
+        <v>1522</v>
+      </c>
+      <c r="J1460" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1461" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A1461" s="1" t="s">
+        <v>1483</v>
+      </c>
+      <c r="B1461" s="1">
+        <v>28.4</v>
+      </c>
+      <c r="C1461" s="1">
+        <v>76</v>
+      </c>
+      <c r="D1461" s="1">
+        <v>1</v>
+      </c>
+      <c r="E1461" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="F1461" s="1">
+        <v>2</v>
+      </c>
+      <c r="G1461" s="1" t="s">
+        <v>1456</v>
+      </c>
+      <c r="H1461" s="6" t="s">
+        <v>1523</v>
+      </c>
+      <c r="I1461" s="6" t="s">
+        <v>1524</v>
+      </c>
+      <c r="J1461" s="7">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="1462" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A1462" s="1" t="s">
+        <v>1484</v>
+      </c>
+      <c r="B1462" s="1">
+        <v>28.4</v>
+      </c>
+      <c r="C1462" s="1">
+        <v>76</v>
+      </c>
+      <c r="D1462" s="1">
+        <v>2</v>
+      </c>
+      <c r="E1462" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="F1462" s="1">
+        <v>2</v>
+      </c>
+      <c r="G1462" s="1" t="s">
+        <v>1461</v>
+      </c>
+      <c r="H1462" s="6" t="s">
+        <v>1525</v>
+      </c>
+      <c r="I1462" s="6" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1462" s="7">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <autoFilter ref="A1:J1462" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="0"/>
+        <filter val="1"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <dataConsolidate/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>